<commit_message>
create smoke check list
</commit_message>
<xml_diff>
--- a/ToDoList_Testing.xlsx
+++ b/ToDoList_Testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>ToDoList - приложение для быстрого управления списками дел. Позволяет сортировать списки по разным критериям: по выполнению, алфавитному порядку и личному предпочтению. Различные значки показывают, все ли задачи из списка завершены.
 Жесты для быстрых действий:
@@ -55,9 +55,6 @@
     <t>S-6</t>
   </si>
   <si>
-    <t>S-7</t>
-  </si>
-  <si>
     <t>Запустить приложение</t>
   </si>
   <si>
@@ -70,34 +67,31 @@
     <t>Добавить задачу в список</t>
   </si>
   <si>
-    <t>Удалить задачу из списка</t>
-  </si>
-  <si>
-    <t>Удалить список</t>
-  </si>
-  <si>
-    <t>Выйти из приложения</t>
-  </si>
-  <si>
-    <t>Приложение загружается быстро или предоставляет пользователю обратную связь на экране</t>
-  </si>
-  <si>
-    <t>На экране корректно отображается созданный список</t>
-  </si>
-  <si>
-    <t>Задача создается и отображается в выбранном списке</t>
-  </si>
-  <si>
-    <t>Задача вычеркивается из списка и помечается чекбоксом</t>
-  </si>
-  <si>
-    <t>Задача удаляется из списка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Список удаляется </t>
-  </si>
-  <si>
     <t>Приложение поддерживает жестовую навигацию для возврата  на главный экран.</t>
+  </si>
+  <si>
+    <t>Установить приложение</t>
+  </si>
+  <si>
+    <t>Приложение скачивается из Google Play, установка проходит без сбоев и ошибок.</t>
+  </si>
+  <si>
+    <t>Приложение загружается быстро или предоставляет пользователю обратную связь на экране. Материалы приложения и метаданные являются полными и точными, отражают основные возможности приложения.</t>
+  </si>
+  <si>
+    <t>На главном экране приложения отображается созданный список.</t>
+  </si>
+  <si>
+    <t>В текущем списке отображается созданная задача.</t>
+  </si>
+  <si>
+    <t>Название выбранной задачи зачеркнуто в текущем списке, чекбокс отмечен.</t>
+  </si>
+  <si>
+    <t>Свернуть приложение</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -126,7 +120,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +130,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,12 +167,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -189,6 +186,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -198,6 +210,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
@@ -498,123 +511,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="D5" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="1"/>
+      <c r="D9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
create critical pass check list
</commit_message>
<xml_diff>
--- a/ToDoList_Testing.xlsx
+++ b/ToDoList_Testing.xlsx
@@ -12,12 +12,12 @@
     <sheet name="Regression Testing" sheetId="3" r:id="rId3"/>
     <sheet name="E2E Testing" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>ToDoList - приложение для быстрого управления списками дел. Позволяет сортировать списки по разным критериям: по выполнению, алфавитному порядку и личному предпочтению. Различные значки показывают, все ли задачи из списка завершены.
 Жесты для быстрых действий:
@@ -133,9 +133,6 @@
     <t>Кликабельность кнопок</t>
   </si>
   <si>
-    <t>Все кнопки кликабельны и выполняют отрабатывают согласно заявленному функционалу</t>
-  </si>
-  <si>
     <t>Создать несколько списков</t>
   </si>
   <si>
@@ -179,13 +176,79 @@
   </si>
   <si>
     <t>Заблокировать/разблокировать экран с запущенным приложением</t>
+  </si>
+  <si>
+    <t>Выполнить все задачи из списка</t>
+  </si>
+  <si>
+    <t>Все задачи из текущего списка зачеркнуты и отмечены чекбоксом. Напротив списка стоит зачок "галочки".</t>
+  </si>
+  <si>
+    <t>Push-уведомления (звонок, СМС, будильник, другое приложение и тд.), всплывающие окна при работе в приложении</t>
+  </si>
+  <si>
+    <t>Push-уведомления от ToDoList</t>
+  </si>
+  <si>
+    <t>При нажатии на уведомление пользователь должен быть перенаправлен на экран в  ToDoList приложении, который непосредственно связан с этим уведомлением и позволяет ему предпринять немедленные действия.</t>
+  </si>
+  <si>
+    <t>После прерывания работы приложение сохраняет состояние пользователя или приложения и предотвращает случайную потерю данных.</t>
+  </si>
+  <si>
+    <t>Все кнопки приложения кликабельны и  отрабатывают согласно заявленному функционалу</t>
+  </si>
+  <si>
+    <t>Сменить ориентацию</t>
+  </si>
+  <si>
+    <t>Свайпнуть верхнюю шторку</t>
+  </si>
+  <si>
+    <t>Свайпнуть нижнюю шторку</t>
+  </si>
+  <si>
+    <t>Приложение поддерживает и правильно обрабатывает как альбомную, так и книжную ориентацию: ориентации раскрывают в основном одни и те же функции и действия и сохраняют функциональный паритет; допускаются незначительные изменения в содержании или представлениях.</t>
+  </si>
+  <si>
+    <t>Разрешение на права доступа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Приложение запрашивает только абсолютно минимальное количество разрешений, которое ему необходимо для поддержки своего варианта использования. </t>
+  </si>
+  <si>
+    <t>Клавиатура показывается при наведении фокуса в текстовое поле, все кнопки кликабельны, кнопки действий «Готово» или « Далее» работают в соответствии с заявленным функционалом</t>
+  </si>
+  <si>
+    <t>Экранная клавиатура</t>
+  </si>
+  <si>
+    <t>Светлая/темная тема</t>
+  </si>
+  <si>
+    <t>Содержимое приложения и все веб-содержимое, на которое ссылается приложение, поддерживают светлую и темную тему .</t>
+  </si>
+  <si>
+    <t>Прерывание работы</t>
+  </si>
+  <si>
+    <t>Системные элементы</t>
+  </si>
+  <si>
+    <t>Тестирование безопасности</t>
+  </si>
+  <si>
+    <t>Политика конфидециальности</t>
+  </si>
+  <si>
+    <t>Все конфиденциальные данные хранятся во внутренней памяти приложения. Никакие личные или конфиденциальные пользовательские данные не записываются в системный журнал или журнал приложения.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,8 +284,17 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -341,27 +419,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -386,19 +477,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -722,12 +813,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -747,13 +838,13 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -767,7 +858,7 @@
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -781,7 +872,7 @@
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -795,7 +886,7 @@
       <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -809,7 +900,7 @@
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -823,7 +914,7 @@
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -843,10 +934,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,12 +949,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -880,76 +971,76 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="25"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="25"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -961,39 +1052,39 @@
       <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" s="24" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+    </row>
+    <row r="12" spans="1:4" s="15" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="22"/>
+      <c r="C12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1002,12 +1093,12 @@
         <v>8</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1021,109 +1112,238 @@
       <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="23"/>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="23"/>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="23"/>
+        <v>47</v>
+      </c>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="C21" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+    </row>
+    <row r="23" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="5" t="s">
+    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="26"/>
-    </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="5" t="s">
+      <c r="C26" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="26"/>
-    </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="26"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="27"/>
+      <c r="B29" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+    </row>
+    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A35:D35"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
create bug reports ToDoList
</commit_message>
<xml_diff>
--- a/ToDoList_Testing.xlsx
+++ b/ToDoList_Testing.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke Testing" sheetId="1" r:id="rId1"/>
     <sheet name="Critical Pass Testing" sheetId="2" r:id="rId2"/>
-    <sheet name="Regression Testing" sheetId="3" r:id="rId3"/>
-    <sheet name="E2E Testing" sheetId="5" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="6" r:id="rId3"/>
+    <sheet name="Regression Testing" sheetId="3" r:id="rId4"/>
+    <sheet name="E2E Testing" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="212">
   <si>
     <t>ToDoList - приложение для быстрого управления списками дел. Позволяет сортировать списки по разным критериям: по выполнению, алфавитному порядку и личному предпочтению. Различные значки показывают, все ли задачи из списка завершены.
 Жесты для быстрых действий:
@@ -496,10 +497,6 @@
     <t>ToDoList does not connect to the network and the data is saved only on your device. This application does not premission and waives advertising and tracking mechanisms.</t>
   </si>
   <si>
-    <t>Pixel 3a API 30
-Android 11.0 Google Play</t>
-  </si>
-  <si>
     <t>Восстановить задачу из списка, нажав кнопку "UNDO"</t>
   </si>
   <si>
@@ -534,6 +531,139 @@
   </si>
   <si>
     <t>C-53</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Trivial</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Enviroment</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Device: Pixel 3a API 30
+OS: Android 11.0 Google Play</t>
+  </si>
+  <si>
+    <t>BC-48</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "CANCEL"  отменяется создание списка и отображается сообщение "Operacion cancelada", а должно  "Operation cancel".</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "CANCEL"  отменяется создание списка и отображается сообщение "Operacion cancelada".</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>При создании новой задачи не предусмотрена возможность отмены создания задачи (отсутствует кнопка "CANCEL").</t>
+  </si>
+  <si>
+    <t>1. На главном экране нажать на плавающую кнопку действия FAB для добавления нового списка.
+2. При появлении всплывающего текстового окна нажать на кнопку "CANCEL".</t>
+  </si>
+  <si>
+    <t>1. В выбранном списке нажать на плавающую кнопку действия FAB для добавления новой задачи.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>BC-49</t>
+  </si>
+  <si>
+    <t>BC-10</t>
+  </si>
+  <si>
+    <t>При сортировке списков по выполнению не учитывается процент выполненния задач в каждом из списков.</t>
+  </si>
+  <si>
+    <t>1. Создать несколько списков.
+2. В некоторых списках создать по несколько задач.
+3. Пометить некоторые задачи, как выполненные.</t>
+  </si>
+  <si>
+    <t>1. Отсортировать задачи по выполнимости, нажав на кнопку "By not done".</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "By not done"  списки задач сортируются по проценту выполнимости снизу вверх.</t>
+  </si>
+  <si>
+    <t>При нажатии на кнопку "By not done"  списки задач некорректно сортируются по проценту выполнимости снизу вверх.</t>
+  </si>
+  <si>
+    <t>При нажатии кнопки "UNDO", удаленный список восстанавливается и отображается на главном экране.</t>
+  </si>
+  <si>
+    <t>При нажатии кнопки "UNDO", все удаленные списки восстанавливаются и отображаются на главном экране.</t>
+  </si>
+  <si>
+    <t>BC-50</t>
+  </si>
+  <si>
+    <t>При удалении задачи из списка не появляется кнопка "UNDO" для ее быстрого восстановления.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Создать список.
+2. Создать задачу в текущем списке.
+</t>
+  </si>
+  <si>
+    <t>1. Смахнуть вправо для удаления задачи.</t>
+  </si>
+  <si>
+    <t>При удалении задачи из списка появляется кнопка "UNDO" с помощью которой можно восстановить только что удаленное задание из текущего списка.</t>
+  </si>
+  <si>
+    <t>При удалении задачи из списка не появляется кнопка "UNDO" с помощью которой можно восстановить только что удаленное задание из текущего списка.</t>
+  </si>
+  <si>
+    <t>BC-53</t>
+  </si>
+  <si>
+    <t>При удалении всех списков не появляется кнопка "UNDO" для их быстрого восстановления.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Создать несколько списков.
+</t>
+  </si>
+  <si>
+    <t>1. Нажать на кнопку "Remove all".</t>
+  </si>
+  <si>
+    <t>При удалении всех списков появляется кнопка "UNDO" с помощью которой можно восстановить только что удаленные списки.</t>
+  </si>
+  <si>
+    <t>При удалении всех списков не появляется кнопка "UNDO" с помощью которой можно восстановить только что удаленные списки.</t>
   </si>
 </sst>
 </file>
@@ -577,7 +707,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +741,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -784,12 +920,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -840,6 +970,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,120 +1029,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1904999</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>114070</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>502003</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>22489</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8139544" y="8216505"/>
-          <a:ext cx="1714277" cy="3767899"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>509315</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>111331</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>459815</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>24741</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9861133" y="8213766"/>
-          <a:ext cx="1768909" cy="3772890"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>453296</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>111331</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>388744</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>37111</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11623523" y="8213766"/>
-          <a:ext cx="1753857" cy="3785260"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>213227</xdr:colOff>
       <xdr:row>39</xdr:row>
@@ -992,7 +1038,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>531916</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>449337</xdr:rowOff>
+      <xdr:rowOff>449336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1002,7 +1048,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1019,22 +1065,179 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>222662</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>61850</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>669481</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1485900" y="3714750"/>
+          <a:ext cx="1466850" cy="574231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>971550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8791575" y="2562225"/>
+          <a:ext cx="1647825" cy="3538953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>11224</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112597</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Рисунок 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11224" y="11287125"/>
+          <a:ext cx="1406298" cy="3076576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>100870</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1533042</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Рисунок 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1405795" y="11287184"/>
+          <a:ext cx="1432172" cy="3076516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1533538</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>320694</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Рисунок 9"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1047,84 +1250,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8139545" y="7904513"/>
-          <a:ext cx="2041072" cy="618506"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>197923</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>235033</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>61851</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>497778</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Рисунок 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8337468" y="7743702"/>
-          <a:ext cx="1682338" cy="658589"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>170592</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>544286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>401180</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>293647</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Рисунок 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10734683" y="6073734"/>
-          <a:ext cx="2048997" cy="4400530"/>
+          <a:off x="2838463" y="11296649"/>
+          <a:ext cx="1368431" cy="3076575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1438,12 +1565,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
@@ -1570,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:D30"/>
+    <sheetView topLeftCell="A19" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,21 +1709,21 @@
     <col min="4" max="4" width="28.5703125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1613,12 +1740,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
     </row>
     <row r="5" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1725,12 +1852,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -1762,13 +1889,13 @@
     </row>
     <row r="16" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>162</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>163</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>156</v>
@@ -1790,13 +1917,13 @@
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>156</v>
@@ -1886,14 +2013,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="C25" s="23"/>
+        <v>158</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>204</v>
+      </c>
       <c r="D25" s="22" t="s">
         <v>156</v>
       </c>
@@ -1912,19 +2041,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="12"/>
+        <v>159</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>154</v>
@@ -1936,25 +2069,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="C29" s="23"/>
+        <v>160</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>199</v>
+      </c>
       <c r="D29" s="22" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
     </row>
     <row r="31" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2019,7 +2154,7 @@
       <c r="B35" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="38" t="s">
         <v>59</v>
       </c>
       <c r="D35" s="12" t="s">
@@ -2033,7 +2168,7 @@
       <c r="B36" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="41"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="12" t="s">
         <v>25</v>
       </c>
@@ -2045,7 +2180,7 @@
       <c r="B37" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="41"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="12" t="s">
         <v>25</v>
       </c>
@@ -2057,7 +2192,7 @@
       <c r="B38" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="41"/>
+      <c r="C38" s="39"/>
       <c r="D38" s="12" t="s">
         <v>25</v>
       </c>
@@ -2069,7 +2204,7 @@
       <c r="B39" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="39"/>
       <c r="D39" s="12" t="s">
         <v>25</v>
       </c>
@@ -2081,7 +2216,7 @@
       <c r="B40" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="41"/>
+      <c r="C40" s="39"/>
       <c r="D40" s="12" t="s">
         <v>25</v>
       </c>
@@ -2093,7 +2228,7 @@
       <c r="B41" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="41"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="22" t="s">
         <v>156</v>
       </c>
@@ -2105,7 +2240,7 @@
       <c r="B42" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="41"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="12" t="s">
         <v>25</v>
       </c>
@@ -2117,7 +2252,7 @@
       <c r="B43" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="41"/>
+      <c r="C43" s="39"/>
       <c r="D43" s="12" t="s">
         <v>25</v>
       </c>
@@ -2129,7 +2264,7 @@
       <c r="B44" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="42"/>
+      <c r="C44" s="40"/>
       <c r="D44" s="12" t="s">
         <v>25</v>
       </c>
@@ -2153,7 +2288,7 @@
       <c r="B46" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="43" t="s">
+      <c r="C46" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D46" s="18"/>
@@ -2165,7 +2300,7 @@
       <c r="B47" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="43"/>
+      <c r="C47" s="41"/>
       <c r="D47" s="18"/>
     </row>
     <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2175,7 +2310,7 @@
       <c r="B48" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="43"/>
+      <c r="C48" s="41"/>
       <c r="D48" s="18"/>
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2185,16 +2320,16 @@
       <c r="B49" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="43"/>
+      <c r="C49" s="41"/>
       <c r="D49" s="18"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="32"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
@@ -2265,12 +2400,12 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="s">
+      <c r="A56" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="30"/>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
@@ -2279,7 +2414,7 @@
       <c r="B57" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="40" t="s">
+      <c r="C57" s="38" t="s">
         <v>96</v>
       </c>
       <c r="D57" s="12" t="s">
@@ -2293,7 +2428,7 @@
       <c r="B58" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="42"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="12" t="s">
         <v>25</v>
       </c>
@@ -2305,7 +2440,7 @@
       <c r="B59" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="38" t="s">
         <v>97</v>
       </c>
       <c r="D59" s="12" t="s">
@@ -2319,7 +2454,7 @@
       <c r="B60" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="42"/>
+      <c r="C60" s="40"/>
       <c r="D60" s="12" t="s">
         <v>25</v>
       </c>
@@ -2339,12 +2474,12 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="30"/>
     </row>
     <row r="63" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
@@ -2356,7 +2491,7 @@
       <c r="C63" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="26" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2370,15 +2505,15 @@
       <c r="C64" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="29"/>
+      <c r="D64" s="27"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
     </row>
     <row r="66" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
@@ -2461,6 +2596,412 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="48"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="D6" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="D7" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="42"/>
+      <c r="D13" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="42"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" s="42"/>
+      <c r="D18" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="42"/>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" s="42"/>
+      <c r="D25" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E25" s="42"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="45" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="42"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2476,20 +3017,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2506,12 +3047,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -2675,12 +3216,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,20 +3233,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">

</xml_diff>